<commit_message>
Primera version funcional sin metricas
</commit_message>
<xml_diff>
--- a/Planteo.xlsx
+++ b/Planteo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson Campos\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Cosas\Desktop\Ejercicio309\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AA1E4DE-5D69-4B8A-B4EE-2FBFEC2A7CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCC043A-1A86-41D5-8FD8-A93FE72B6CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4905" windowWidth="29040" windowHeight="15840" xr2:uid="{E22D0D24-C983-48C1-8C76-FCDF2B098E41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E22D0D24-C983-48C1-8C76-FCDF2B098E41}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Evento</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Exponencial</t>
   </si>
   <si>
-    <t>30 llamadas por hora</t>
-  </si>
-  <si>
     <t>Llegada Ambulancia</t>
   </si>
   <si>
@@ -192,6 +189,30 @@
   </si>
   <si>
     <t>Estado 8</t>
+  </si>
+  <si>
+    <t>Ambulancia (P)</t>
+  </si>
+  <si>
+    <t>Libre (L)</t>
+  </si>
+  <si>
+    <t>Yendo (Y)</t>
+  </si>
+  <si>
+    <t>Volviendo (V)</t>
+  </si>
+  <si>
+    <t>Paciente (T)</t>
+  </si>
+  <si>
+    <t>Esperando Atencion (Ea)</t>
+  </si>
+  <si>
+    <t>En Traslado (Et)</t>
+  </si>
+  <si>
+    <t>30 llamadas por hora; (30/60) llamadas por min</t>
   </si>
 </sst>
 </file>
@@ -386,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -396,11 +417,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -432,20 +462,48 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,13 +821,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE91B4E-5954-41FE-A8F7-36317B665F73}">
   <dimension ref="A2:AL15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE15" sqref="AE15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -783,282 +842,342 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="3"/>
-      <c r="K3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="14"/>
+      <c r="K3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="17"/>
+      <c r="Q3" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="26"/>
+      <c r="S3" s="3"/>
+      <c r="U3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V3" s="2"/>
+      <c r="W3" s="3"/>
     </row>
     <row r="4" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="5"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="17"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="20"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" s="28"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="32"/>
     </row>
-    <row r="5" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="5"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="S5" s="28"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="W5" s="34"/>
     </row>
     <row r="6" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="9"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="5"/>
-      <c r="K6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="20"/>
+      <c r="K6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="23"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="30"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="9"/>
+      <c r="B7" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="36"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
-      <c r="K8" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="23"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="5"/>
+      <c r="K8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="12"/>
+    </row>
+    <row r="9" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="K14" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="25"/>
-      <c r="V14" s="25"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="25"/>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="25"/>
-      <c r="AB14" s="25"/>
-      <c r="AE14" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF14" s="25"/>
-      <c r="AG14" s="25"/>
-      <c r="AH14" s="25"/>
-      <c r="AI14" s="25"/>
-      <c r="AJ14" s="25"/>
-      <c r="AK14" s="25"/>
-      <c r="AL14" s="25"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AE14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF14" s="13"/>
+      <c r="AG14" s="13"/>
+      <c r="AH14" s="13"/>
+      <c r="AI14" s="13"/>
+      <c r="AJ14" s="13"/>
+      <c r="AK14" s="13"/>
+      <c r="AL14" s="13"/>
     </row>
     <row r="15" spans="1:38" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="E15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="F15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="G15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="24" t="s">
+      <c r="I15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="24" t="s">
+      <c r="J15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="24" t="s">
+      <c r="M15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M15" s="24" t="s">
+      <c r="N15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="N15" s="24" t="s">
+      <c r="O15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O15" s="24" t="s">
+      <c r="P15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="P15" s="24" t="s">
+      <c r="Q15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Q15" s="24" t="s">
+      <c r="R15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="R15" s="24" t="s">
+      <c r="S15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="S15" s="24" t="s">
+      <c r="T15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T15" s="24" t="s">
+      <c r="U15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U15" s="24" t="s">
+      <c r="V15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="V15" s="24" t="s">
+      <c r="W15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="W15" s="24" t="s">
+      <c r="X15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="X15" s="24" t="s">
+      <c r="Y15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="Y15" s="24" t="s">
+      <c r="Z15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="Z15" s="24" t="s">
+      <c r="AA15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AA15" s="24" t="s">
+      <c r="AB15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AB15" s="24" t="s">
+      <c r="AC15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AC15" s="24" t="s">
+      <c r="AD15" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AD15" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE15" s="24" t="s">
+      <c r="AE15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AF15" s="24" t="s">
+      <c r="AG15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AG15" s="24" t="s">
+      <c r="AH15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AH15" s="24" t="s">
+      <c r="AI15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AI15" s="24" t="s">
+      <c r="AJ15" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="AJ15" s="24" t="s">
+      <c r="AK15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AK15" s="24" t="s">
+      <c r="AL15" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="AL15" s="24" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="25">
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="K3:N4"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="F5:G6"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="K14:AB14"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="AE14:AL14"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="K3:N4"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>